<commit_message>
add data to sheet
</commit_message>
<xml_diff>
--- a/Reference Studies - news classification .xlsx
+++ b/Reference Studies - news classification .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>ML Algorithm</t>
+  </si>
+  <si>
+    <t>Deep Learning AL</t>
   </si>
   <si>
     <t>Dataset</t>
@@ -67,6 +70,9 @@
     <t>BERTje</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>A dataset was created containing 1,771 Dutch language news articles</t>
   </si>
   <si>
@@ -82,19 +88,39 @@
     <t>Economics, business and politics</t>
   </si>
   <si>
-    <t>news classification using machine learning</t>
-  </si>
-  <si>
-    <t>In the context of Natural Language Processing (NLP), various techniques are employed to process and analyze text data</t>
-  </si>
-  <si>
-    <t>In Natural Language Processing (NLP), the typical approach involves several key processes to analyze and understand text data: Data Collection,Data Preprocessing,Feature Engineering,Model Building,Model Evaluation,Model Deployment</t>
-  </si>
-  <si>
-    <t>a news related dataset which having</t>
-  </si>
-  <si>
-    <t>News Classification Using Machine Learning</t>
+    <t>Spotting fake news in Arabic with Machine and Deep Learning Techniques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The study examines the content of fake news in the Arabic-speaking world through YouTube comments and compares the performance of machine learning and deep learning techniques in detecting fake news.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The study uses preprocessing, classical machine learning, and neural networks </t>
+  </si>
+  <si>
+    <t>Support Vector Machine (SVM), Decision Tree (DT), Multinomial Naive Bayes (MNB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Long Short-Term Memory (LSTM), Bidirectional Long Short-Term Memory (BILSTM), and Convolutional Neural Network (CNN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The study uses an Arabic corpus for fake news analysis, focusing on rumors related to the death of prominent Arab personalities.</t>
+  </si>
+  <si>
+    <t>accuracy, precision,
+and recall</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>The study concludes that both machine learning and deep learning models showed high accuracy in detecting fake news in Arabic, with the SVM classifier performing the best among the machine learning models and the BiLSTM classifier performing the best among the deep learning models.</t>
+  </si>
+  <si>
+    <t>Fake , real</t>
+  </si>
+  <si>
+    <t>Spotting fake news in Arabic with Machine and Deep Learning Techniques - Archive ouverte HAL</t>
   </si>
   <si>
     <t>Multi‑category news classifcation using Support Vector Machine based classifers</t>
@@ -192,6 +218,21 @@
   </si>
   <si>
     <t>non</t>
+  </si>
+  <si>
+    <t>news classification using machine learning</t>
+  </si>
+  <si>
+    <t>In the context of Natural Language Processing (NLP), various techniques are employed to process and analyze text data</t>
+  </si>
+  <si>
+    <t>In Natural Language Processing (NLP), the typical approach involves several key processes to analyze and understand text data: Data Collection,Data Preprocessing,Feature Engineering,Model Building,Model Evaluation,Model Deployment</t>
+  </si>
+  <si>
+    <t>a news related dataset which having</t>
+  </si>
+  <si>
+    <t>News Classification Using Machine Learning</t>
   </si>
 </sst>
 </file>
@@ -235,8 +276,10 @@
       <name val="Roboto"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -285,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -325,32 +368,29 @@
     <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +617,10 @@
     <col customWidth="1" min="4" max="4" width="53.75"/>
     <col customWidth="1" min="5" max="5" width="25.63"/>
     <col customWidth="1" min="6" max="6" width="27.63"/>
-    <col customWidth="1" min="7" max="8" width="25.25"/>
-    <col customWidth="1" min="9" max="9" width="25.63"/>
-    <col customWidth="1" min="10" max="10" width="25.5"/>
-    <col customWidth="1" min="11" max="12" width="25.25"/>
+    <col customWidth="1" min="7" max="9" width="25.25"/>
+    <col customWidth="1" min="10" max="10" width="25.63"/>
+    <col customWidth="1" min="11" max="11" width="25.5"/>
+    <col customWidth="1" min="12" max="13" width="25.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -620,418 +660,475 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="63.0" customHeight="1">
       <c r="A2" s="3">
         <v>1.0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5">
         <v>2020.0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" ht="59.25" customHeight="1">
-      <c r="A3" s="13">
+    </row>
+    <row r="3" ht="63.0" customHeight="1">
+      <c r="A3" s="3">
         <v>2.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5">
-        <v>2021.0</v>
+        <v>2023.0</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="F3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" ht="62.25" customHeight="1">
-      <c r="A4" s="13">
+      <c r="A4" s="3">
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5">
         <v>2020.0</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>27</v>
+      <c r="D4" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" ht="62.25" customHeight="1">
-      <c r="A5" s="13">
+      <c r="A5" s="3">
         <v>4.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5">
         <v>2018.0</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>38</v>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" ht="47.25" customHeight="1">
-      <c r="A6" s="13">
+      <c r="A6" s="3">
         <v>5.0</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>46</v>
+      <c r="B6" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C6" s="5">
         <v>2021.0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" ht="45.75" customHeight="1">
-      <c r="A7" s="13">
+        <v>61</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" ht="59.25" customHeight="1">
+      <c r="A7" s="3">
         <v>6.0</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="13">
+      <c r="B7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" ht="47.25" customHeight="1">
+      <c r="A8" s="16">
         <v>7.0</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="13">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" ht="48.0" customHeight="1">
+      <c r="A9" s="16">
         <v>8.0</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="13">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" ht="45.0" customHeight="1">
+      <c r="A10" s="20">
         <v>9.0</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11">
-      <c r="A11" s="13">
+      <c r="A11" s="20">
         <v>10.0</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12">
-      <c r="A12" s="13">
+      <c r="A12" s="20">
         <v>11.0</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
     </row>
     <row r="13">
-      <c r="A13" s="13">
+      <c r="A13" s="20">
         <v>12.0</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14">
-      <c r="A14" s="13">
+      <c r="A14" s="20">
         <v>13.0</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15">
-      <c r="A15" s="13">
+      <c r="A15" s="20">
         <v>14.0</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="20">
         <v>15.0</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17">
-      <c r="A17" s="13">
+      <c r="A17" s="20">
         <v>16.0</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18">
-      <c r="A18" s="13">
+      <c r="A18" s="20">
         <v>17.0</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19">
-      <c r="A19" s="13">
+      <c r="A19" s="20">
         <v>18.0</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
     </row>
     <row r="20">
-      <c r="A20" s="13">
+      <c r="A20" s="20">
         <v>19.0</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="L2"/>
-    <hyperlink r:id="rId2" ref="L3"/>
-    <hyperlink r:id="rId3" ref="L4"/>
-    <hyperlink display="https://docs.google.com/spreadsheets/d/1Owl_aRtzi-hwGqN9q_bLtI4xIdZupBKMvXjX4m_D1Lo/edit#gid=0&amp;range=D5" location="'الورقة1'!D5" ref="L5"/>
+    <hyperlink r:id="rId1" ref="M2"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M4"/>
+    <hyperlink display="https://docs.google.com/spreadsheets/d/1Owl_aRtzi-hwGqN9q_bLtI4xIdZupBKMvXjX4m_D1Lo/edit#gid=0&amp;range=D5" location="'الورقة1'!D5" ref="M5"/>
+    <hyperlink r:id="rId4" ref="M7"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
News Classification - User InterFace v.1.1.0
</commit_message>
<xml_diff>
--- a/Reference Studies - news classification .xlsx
+++ b/Reference Studies - news classification .xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unavercity\NC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDBABAE-A3A3-4A7C-BC00-4B199E114EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="الورقة1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="الورقة2" sheetId="2" r:id="rId5"/>
+    <sheet name="الورقة1" sheetId="1" r:id="rId1"/>
+    <sheet name="الورقة2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -468,39 +477,42 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -508,47 +520,55 @@
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
@@ -558,7 +578,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -592,7 +612,13 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -606,6 +632,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -614,11 +641,14 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -628,143 +658,128 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+  <cellXfs count="29">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -954,36 +969,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.88"/>
-    <col customWidth="1" min="2" max="2" width="65.63"/>
-    <col customWidth="1" min="3" max="3" width="7.0"/>
-    <col customWidth="1" min="4" max="4" width="53.75"/>
-    <col customWidth="1" min="5" max="5" width="25.63"/>
-    <col customWidth="1" min="6" max="6" width="27.63"/>
-    <col customWidth="1" min="7" max="9" width="25.25"/>
-    <col customWidth="1" min="10" max="10" width="25.63"/>
-    <col customWidth="1" min="11" max="11" width="25.5"/>
-    <col customWidth="1" min="12" max="12" width="25.25"/>
-    <col customWidth="1" min="13" max="13" width="38.13"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="53.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="9" width="25.21875" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" customWidth="1"/>
+    <col min="12" max="12" width="25.21875" customWidth="1"/>
+    <col min="13" max="13" width="88.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" ht="13.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -993,623 +1011,624 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" ht="81.0" customHeight="1">
-      <c r="A2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:13" ht="81" customHeight="1">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7">
-        <v>2021.0</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="5">
+        <v>2021</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" ht="84.0" customHeight="1">
-      <c r="A3" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:13" ht="84" customHeight="1">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7">
-        <v>2020.0</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="5">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="13" t="s">
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" ht="84.0" customHeight="1">
-      <c r="A4" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:13" ht="84" customHeight="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7">
-        <v>2018.0</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="11" t="s">
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" ht="67.5" customHeight="1">
-      <c r="A5" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:13" ht="67.5" customHeight="1">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="7">
-        <v>2019.0</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="5">
+        <v>2019</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="18" t="s">
+      <c r="G5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" ht="82.5" customHeight="1">
-      <c r="A6" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:13" ht="82.5" customHeight="1">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="7">
-        <v>2021.0</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="5">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="15" t="s">
+      <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" ht="84.0" customHeight="1">
-      <c r="A7" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:13" ht="84" customHeight="1">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="7">
-        <v>2023.0</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="5">
+        <v>2023</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" ht="88.5" customHeight="1">
-      <c r="A8" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:13" ht="88.5" customHeight="1">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="7">
-        <v>2020.0</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="5">
+        <v>2020</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="21" t="s">
+      <c r="G8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" ht="82.5" customHeight="1">
-      <c r="A9" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="1:13" ht="82.5" customHeight="1">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="7">
-        <v>2019.0</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="5">
+        <v>2019</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="13" t="s">
+      <c r="F9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="13" t="s">
+      <c r="J9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="24" t="s">
+      <c r="L9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" ht="84.0" customHeight="1">
-      <c r="A10" s="5">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="1:13" ht="84" customHeight="1">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="7">
-        <v>2021.0</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="5">
+        <v>2021</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="H10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" ht="88.5" customHeight="1">
-      <c r="A11" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="27" t="s">
+    <row r="11" spans="1:13" ht="88.5" customHeight="1">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="7">
-        <v>2024.0</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="5">
+        <v>2024</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="13" t="s">
+      <c r="H11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="28" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="M2"/>
-    <hyperlink r:id="rId2" ref="M3"/>
-    <hyperlink r:id="rId3" location="read" ref="M4"/>
-    <hyperlink r:id="rId4" ref="M5"/>
-    <hyperlink r:id="rId5" ref="M6"/>
-    <hyperlink r:id="rId6" ref="M7"/>
-    <hyperlink r:id="rId7" ref="H8"/>
-    <hyperlink r:id="rId8" ref="M8"/>
-    <hyperlink r:id="rId9" ref="H9"/>
-    <hyperlink r:id="rId10" ref="M9"/>
-    <hyperlink r:id="rId11" location="references" ref="M10"/>
-    <hyperlink r:id="rId12" ref="M11"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M4" r:id="rId3" location="read" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M10" r:id="rId11" location="references" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="21.75"/>
-    <col customWidth="1" min="7" max="7" width="25.25"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:7" ht="13.2">
+      <c r="A1" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:7" ht="52.8">
+      <c r="A2" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="32">
-        <v>2021.0</v>
-      </c>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="25">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="25" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:7" ht="105.6">
+      <c r="A3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="32">
-        <v>2020.0</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="25">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" ht="90.75" customHeight="1">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:7" ht="90.75" customHeight="1">
+      <c r="A4" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="32">
-        <v>2018.0</v>
-      </c>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="25">
+        <v>2018</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="25" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" ht="82.5" customHeight="1">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:7" ht="82.5" customHeight="1">
+      <c r="A5" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="32">
-        <v>2023.0</v>
-      </c>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="25">
+        <v>2023</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="25" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" ht="51.75" customHeight="1">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A6" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="32">
-        <v>2024.0</v>
-      </c>
-      <c r="C6" s="33" t="s">
+      <c r="B6" s="25">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="25" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C6"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>